<commit_message>
queries in real dataset
</commit_message>
<xml_diff>
--- a/encodingTimeGroupByNew.xlsx
+++ b/encodingTimeGroupByNew.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Documents\Diplomatiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0063F0AA-4A17-4E6B-A381-BC96A3A83E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BEB404-073C-49E4-A580-66423AAA4928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{677757BE-B749-4A72-AE97-9E6E71039D15}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="uniform" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,8 +71,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -105,8 +106,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -5983,8 +5984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7442891D-67CF-4F9D-9D7F-238AB0258C01}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>